<commit_message>
highlighting best price, api filtering
code needs restructuring
</commit_message>
<xml_diff>
--- a/testfiles/Wooi Nee - Keri MPNs.xlsx
+++ b/testfiles/Wooi Nee - Keri MPNs.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\SRX\plm\testfiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlew\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B25B28A-C415-46F4-A0F8-AC8D88D162FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CEB84D07-5BF9-4341-A0F9-C0B5A76615F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32910" yWindow="300" windowWidth="23925" windowHeight="13650" xr2:uid="{22B7E0FC-6997-4213-AF62-654D8F91863B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10536" xr2:uid="{22B7E0FC-6997-4213-AF62-654D8F91863B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$98</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$102</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="346">
   <si>
     <t>Component number</t>
   </si>
@@ -255,6 +255,12 @@
     <t>RES, 2.80K OHM 1/4W 1% 1206</t>
   </si>
   <si>
+    <t>LFK02019020</t>
+  </si>
+  <si>
+    <t>NXT Controller FW V2.05.80</t>
+  </si>
+  <si>
     <t>LFK36024001</t>
   </si>
   <si>
@@ -297,6 +303,12 @@
     <t>IC, DS1708SESA</t>
   </si>
   <si>
+    <t>LFK41057001</t>
+  </si>
+  <si>
+    <t>IC, SN74LV08ADBR</t>
+  </si>
+  <si>
     <t>LFK41059001</t>
   </si>
   <si>
@@ -603,6 +615,12 @@
     <t>TRANSORB,SA15A</t>
   </si>
   <si>
+    <t>LFK36052001</t>
+  </si>
+  <si>
+    <t>LED,GREEN</t>
+  </si>
+  <si>
     <t>LFK36056001</t>
   </si>
   <si>
@@ -627,6 +645,12 @@
     <t>Ferrite 120Ohm 25% 100MHz0603</t>
   </si>
   <si>
+    <t>LFK53045001</t>
+  </si>
+  <si>
+    <t>RELAY, SPDT 12V DC</t>
+  </si>
+  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -759,6 +783,12 @@
     <t>RC1206FR-072K8L</t>
   </si>
   <si>
+    <t>CYPRESS</t>
+  </si>
+  <si>
+    <t>S29GL064S80TFIV60</t>
+  </si>
+  <si>
     <t>DIODES INC</t>
   </si>
   <si>
@@ -792,6 +822,9 @@
     <t>STM708SM6F</t>
   </si>
   <si>
+    <t>SN74LV08ADBR</t>
+  </si>
+  <si>
     <t>MICROCHIP</t>
   </si>
   <si>
@@ -1020,6 +1053,9 @@
     <t>LITE-ON</t>
   </si>
   <si>
+    <t>LTST-C150GKT</t>
+  </si>
+  <si>
     <t>LTST-C150KRKT</t>
   </si>
   <si>
@@ -1030,6 +1066,12 @@
   </si>
   <si>
     <t>BLM18PG121SN1D</t>
+  </si>
+  <si>
+    <t>NAIS</t>
+  </si>
+  <si>
+    <t>JS1-12V-F</t>
   </si>
   <si>
     <t>Need qty</t>
@@ -1440,23 +1482,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86D68A4A-C8DC-4018-8E4A-C079D2D3962D}">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="27.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="17.20703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.3671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.3125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.62890625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1464,16 +1506,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>196</v>
+        <v>204</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1481,16 +1523,16 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="E2" s="2">
         <v>9000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -1498,16 +1540,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="E3" s="2">
         <v>14000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -1515,16 +1557,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="E4" s="2">
         <v>9000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1532,16 +1574,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>205</v>
+        <v>213</v>
       </c>
       <c r="E5" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -1549,16 +1591,16 @@
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E6" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -1566,16 +1608,16 @@
         <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>208</v>
+        <v>216</v>
       </c>
       <c r="E7" s="2">
         <v>7000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -1583,16 +1625,16 @@
         <v>15</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>209</v>
+        <v>217</v>
       </c>
       <c r="E8" s="2">
         <v>12000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1600,16 +1642,16 @@
         <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="E9" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1617,16 +1659,16 @@
         <v>19</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E10" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1634,16 +1676,16 @@
         <v>21</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="E11" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1651,16 +1693,16 @@
         <v>23</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="E12" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1668,16 +1710,16 @@
         <v>25</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="E13" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1685,16 +1727,16 @@
         <v>27</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="E14" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
@@ -1702,16 +1744,16 @@
         <v>29</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="E15" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
@@ -1719,16 +1761,16 @@
         <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>218</v>
+        <v>226</v>
       </c>
       <c r="E16" s="2">
         <v>10000</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -1736,16 +1778,16 @@
         <v>33</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>219</v>
+        <v>227</v>
       </c>
       <c r="E17" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1753,16 +1795,16 @@
         <v>35</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>220</v>
+        <v>228</v>
       </c>
       <c r="E18" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1770,16 +1812,16 @@
         <v>37</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="E19" s="2">
         <v>4000</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1787,16 +1829,16 @@
         <v>39</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>222</v>
+        <v>230</v>
       </c>
       <c r="E20" s="2">
         <v>6000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1804,16 +1846,16 @@
         <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="E21" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1821,16 +1863,16 @@
         <v>43</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
       <c r="E22" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1838,16 +1880,16 @@
         <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="E23" s="2">
         <v>26000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
@@ -1855,16 +1897,16 @@
         <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>227</v>
+        <v>235</v>
       </c>
       <c r="E24" s="2">
         <v>17000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
@@ -1872,16 +1914,16 @@
         <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="E25" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1889,16 +1931,16 @@
         <v>51</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="E26" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1906,16 +1948,16 @@
         <v>53</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="E27" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
@@ -1923,16 +1965,16 @@
         <v>55</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="E28" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
@@ -1940,16 +1982,16 @@
         <v>57</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>232</v>
+        <v>240</v>
       </c>
       <c r="E29" s="2">
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1957,16 +1999,16 @@
         <v>59</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>233</v>
+        <v>241</v>
       </c>
       <c r="E30" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -1974,16 +2016,16 @@
         <v>61</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="E31" s="2">
         <v>8000</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
@@ -1991,16 +2033,16 @@
         <v>63</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>235</v>
+        <v>243</v>
       </c>
       <c r="E32" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2008,16 +2050,16 @@
         <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="E33" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
@@ -2025,16 +2067,16 @@
         <v>67</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>237</v>
+        <v>245</v>
       </c>
       <c r="E34" s="2">
         <v>9000</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
@@ -2042,16 +2084,16 @@
         <v>69</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>238</v>
+        <v>246</v>
       </c>
       <c r="E35" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -2059,16 +2101,16 @@
         <v>71</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="E36" s="2">
         <v>6000</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2076,16 +2118,16 @@
         <v>73</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>240</v>
+        <v>248</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>241</v>
+        <v>249</v>
       </c>
       <c r="E37" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
@@ -2093,16 +2135,16 @@
         <v>75</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="E38" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
@@ -2110,16 +2152,16 @@
         <v>77</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
       <c r="E39" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
@@ -2127,16 +2169,16 @@
         <v>79</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>246</v>
+        <v>254</v>
       </c>
       <c r="E40" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
@@ -2144,16 +2186,16 @@
         <v>81</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="E41" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
@@ -2161,16 +2203,16 @@
         <v>83</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="E42" s="2">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
@@ -2178,16 +2220,16 @@
         <v>85</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
       <c r="E43" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
@@ -2195,16 +2237,16 @@
         <v>87</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>251</v>
+        <v>259</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>252</v>
+        <v>260</v>
       </c>
       <c r="E44" s="2">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
@@ -2212,16 +2254,16 @@
         <v>89</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="E45" s="2">
-        <v>3500</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
@@ -2229,16 +2271,16 @@
         <v>91</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="E46" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
@@ -2246,16 +2288,16 @@
         <v>93</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="E47" s="2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
@@ -2263,16 +2305,16 @@
         <v>95</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="E48" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
@@ -2280,16 +2322,16 @@
         <v>97</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="E49" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
@@ -2297,16 +2339,16 @@
         <v>99</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="E50" s="2">
         <v>4500</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
@@ -2314,16 +2356,16 @@
         <v>101</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="E51" s="2">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A52" s="2" t="s">
         <v>102</v>
       </c>
@@ -2331,16 +2373,16 @@
         <v>103</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="E52" s="2">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -2348,16 +2390,16 @@
         <v>105</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="E53" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
@@ -2365,16 +2407,16 @@
         <v>107</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="E54" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55" s="2" t="s">
         <v>108</v>
       </c>
@@ -2382,16 +2424,16 @@
         <v>109</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="E55" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
@@ -2399,16 +2441,16 @@
         <v>111</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="E56" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
@@ -2416,16 +2458,16 @@
         <v>113</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="E57" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A58" s="2" t="s">
         <v>114</v>
       </c>
@@ -2433,16 +2475,16 @@
         <v>115</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="E58" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A59" s="2" t="s">
         <v>116</v>
       </c>
@@ -2450,16 +2492,16 @@
         <v>117</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>270</v>
+        <v>281</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="E59" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A60" s="2" t="s">
         <v>118</v>
       </c>
@@ -2467,16 +2509,16 @@
         <v>119</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="E60" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A61" s="2" t="s">
         <v>120</v>
       </c>
@@ -2484,16 +2526,16 @@
         <v>121</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="E61" s="2">
         <v>1000</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A62" s="2" t="s">
         <v>122</v>
       </c>
@@ -2501,16 +2543,16 @@
         <v>123</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="E62" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A63" s="2" t="s">
         <v>124</v>
       </c>
@@ -2518,16 +2560,16 @@
         <v>125</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="E63" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A64" s="2" t="s">
         <v>126</v>
       </c>
@@ -2535,16 +2577,16 @@
         <v>127</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="E64" s="2">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A65" s="2" t="s">
         <v>128</v>
       </c>
@@ -2552,16 +2594,16 @@
         <v>129</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="E65" s="2">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A66" s="2" t="s">
         <v>130</v>
       </c>
@@ -2569,16 +2611,16 @@
         <v>131</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>207</v>
+        <v>295</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="E66" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A67" s="2" t="s">
         <v>132</v>
       </c>
@@ -2586,16 +2628,16 @@
         <v>133</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="E67" s="2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A68" s="2" t="s">
         <v>134</v>
       </c>
@@ -2603,16 +2645,16 @@
         <v>135</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="E68" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A69" s="2" t="s">
         <v>136</v>
       </c>
@@ -2620,16 +2662,16 @@
         <v>137</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="E69" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A70" s="2" t="s">
         <v>138</v>
       </c>
@@ -2637,16 +2679,16 @@
         <v>139</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="E70" s="2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A71" s="2" t="s">
         <v>140</v>
       </c>
@@ -2654,16 +2696,16 @@
         <v>141</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>289</v>
+        <v>224</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="E71" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A72" s="2" t="s">
         <v>142</v>
       </c>
@@ -2671,16 +2713,16 @@
         <v>143</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>295</v>
+        <v>215</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="E72" s="2">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A73" s="2" t="s">
         <v>144</v>
       </c>
@@ -2688,16 +2730,16 @@
         <v>145</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="E73" s="2">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A74" s="2" t="s">
         <v>146</v>
       </c>
@@ -2705,16 +2747,16 @@
         <v>147</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>207</v>
+        <v>306</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="E74" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A75" s="2" t="s">
         <v>148</v>
       </c>
@@ -2722,16 +2764,16 @@
         <v>149</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="E75" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A76" s="2" t="s">
         <v>150</v>
       </c>
@@ -2739,16 +2781,16 @@
         <v>151</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="E76" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A77" s="2" t="s">
         <v>152</v>
       </c>
@@ -2756,16 +2798,16 @@
         <v>153</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="E77" s="2">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A78" s="2" t="s">
         <v>154</v>
       </c>
@@ -2773,16 +2815,16 @@
         <v>155</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="E78" s="2">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A79" s="2" t="s">
         <v>156</v>
       </c>
@@ -2790,16 +2832,16 @@
         <v>157</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="E79" s="2">
-        <v>14000</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A80" s="2" t="s">
         <v>158</v>
       </c>
@@ -2807,16 +2849,16 @@
         <v>159</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>289</v>
+        <v>215</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="E80" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A81" s="2" t="s">
         <v>160</v>
       </c>
@@ -2824,16 +2866,16 @@
         <v>161</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="E81" s="2">
-        <v>42000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A82" s="2" t="s">
         <v>162</v>
       </c>
@@ -2841,16 +2883,16 @@
         <v>163</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="E82" s="2">
         <v>3000</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A83" s="2" t="s">
         <v>164</v>
       </c>
@@ -2858,16 +2900,16 @@
         <v>165</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>216</v>
+        <v>306</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="E83" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A84" s="2" t="s">
         <v>166</v>
       </c>
@@ -2875,16 +2917,16 @@
         <v>167</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E84" s="2">
-        <v>35000</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A85" s="2" t="s">
         <v>168</v>
       </c>
@@ -2892,16 +2934,16 @@
         <v>169</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>216</v>
+        <v>224</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="E85" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A86" s="2" t="s">
         <v>170</v>
       </c>
@@ -2909,16 +2951,16 @@
         <v>171</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>310</v>
+        <v>215</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>311</v>
+        <v>319</v>
       </c>
       <c r="E86" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A87" s="2" t="s">
         <v>172</v>
       </c>
@@ -2926,16 +2968,16 @@
         <v>173</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>312</v>
+        <v>224</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="E87" s="2">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A88" s="2" t="s">
         <v>174</v>
       </c>
@@ -2943,16 +2985,16 @@
         <v>175</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="E88" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A89" s="2" t="s">
         <v>176</v>
       </c>
@@ -2960,16 +3002,16 @@
         <v>177</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="E89" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A90" s="2" t="s">
         <v>178</v>
       </c>
@@ -2977,16 +3019,16 @@
         <v>179</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>319</v>
+        <v>325</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="E90" s="2">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A91" s="2" t="s">
         <v>180</v>
       </c>
@@ -2994,16 +3036,16 @@
         <v>181</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="E91" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A92" s="2" t="s">
         <v>182</v>
       </c>
@@ -3011,16 +3053,16 @@
         <v>183</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>240</v>
+        <v>330</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="E92" s="2">
-        <v>4500</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A93" s="2" t="s">
         <v>184</v>
       </c>
@@ -3028,16 +3070,16 @@
         <v>185</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>280</v>
+        <v>332</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="E93" s="2">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A94" s="2" t="s">
         <v>186</v>
       </c>
@@ -3045,16 +3087,16 @@
         <v>187</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>295</v>
+        <v>250</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="E94" s="2">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A95" s="2" t="s">
         <v>188</v>
       </c>
@@ -3062,16 +3104,16 @@
         <v>189</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>326</v>
+        <v>291</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="E95" s="2">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A96" s="2" t="s">
         <v>190</v>
       </c>
@@ -3079,16 +3121,16 @@
         <v>191</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="E96" s="2">
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A97" s="2" t="s">
         <v>192</v>
       </c>
@@ -3096,16 +3138,16 @@
         <v>193</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>319</v>
+        <v>337</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="E97" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10500</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A98" s="2" t="s">
         <v>194</v>
       </c>
@@ -3113,13 +3155,81 @@
         <v>195</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>318</v>
+        <v>337</v>
       </c>
       <c r="D98" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E98" s="2">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A99" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="E99" s="2">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A100" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="E98" s="2">
+      <c r="D100" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A101" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="E101" s="2">
         <v>500</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A102" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="E102" s="2">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>